<commit_message>
mini project code done
</commit_message>
<xml_diff>
--- a/pythonexcel1.xlsx
+++ b/pythonexcel1.xlsx
@@ -596,19 +596,9 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>99003766</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Jayasimha Reddy Ganapuram</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>jayasimha.ganapuram@ltts.com</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
           <t>Nalanda</t>
@@ -633,91 +623,33 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J2" t="n">
-        <v>21</v>
-      </c>
-      <c r="K2" t="n">
-        <v>2</v>
-      </c>
-      <c r="L2" t="n">
-        <v>9</v>
-      </c>
-      <c r="M2" t="n">
-        <v>60</v>
-      </c>
-      <c r="N2" t="n">
-        <v>63</v>
-      </c>
-      <c r="O2" t="n">
-        <v>55</v>
-      </c>
-      <c r="P2" t="n">
-        <v>37</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>53</v>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-      <c r="S2" t="n">
-        <v>40</v>
-      </c>
-      <c r="T2" t="n">
-        <v>99</v>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>Fresher</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>College</t>
-        </is>
-      </c>
-      <c r="X2" t="n">
-        <v>10000</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>ECE</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>Fairfield Marriot</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>Rajajinagar</t>
-        </is>
-      </c>
-      <c r="AC2" t="n">
-        <v>120</v>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>AP</t>
-        </is>
-      </c>
-      <c r="AE2" t="n">
-        <v>21</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>120</v>
-      </c>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>